<commit_message>
added all basic components
added arduino include paths
added TemperatureSensor
added AutomaticFan
added RCReceiver
added RGBLed
started with StateManager
started with I2CManager
updated Datasheet
added board-pins.txt
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Arduino\projects\AIDrone-RCController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Arduino\projects\AICar-RCController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F7248F-68B9-4255-8669-066F5445C7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281BB22F-1855-4DC2-8A92-26A27D415FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C Get Commands" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Get</t>
   </si>
@@ -49,19 +49,7 @@
     <t>Return (Description)</t>
   </si>
   <si>
-    <t>RC-Receiver User Input Throttle</t>
-  </si>
-  <si>
-    <t>RC-Receiver User Input Steering</t>
-  </si>
-  <si>
     <t>Motor Temperature</t>
-  </si>
-  <si>
-    <t>uint16</t>
-  </si>
-  <si>
-    <t>Pulse Width in Microseconds</t>
   </si>
   <si>
     <t>int16</t>
@@ -94,12 +82,6 @@
   </si>
   <si>
     <t>Write Argument2 (Description)</t>
-  </si>
-  <si>
-    <t>Throttle (ESC Input)</t>
-  </si>
-  <si>
-    <t>Steering (Steer Servo Input)</t>
   </si>
   <si>
     <t>Implemented</t>
@@ -111,36 +93,57 @@
 Timeout of 10 seconds to confirm the mode change via user input. (hold full brake and full left for at least 1 second and then relase to confirm)</t>
   </si>
   <si>
-    <t>Motor Fan Mode</t>
-  </si>
-  <si>
-    <t>0 = Automatic
-1 = Manual</t>
-  </si>
-  <si>
-    <t>Motor Fan Manual Speed</t>
-  </si>
-  <si>
-    <t>0-100% Fan Speed</t>
+    <t>Motor Fan Info</t>
+  </si>
+  <si>
+    <t>Fan Info</t>
+  </si>
+  <si>
+    <t>0-1: Fan Speed (uint8_t)
+1-3: Update Interval Millis (uint16_t)
+3-5: Fan Off Temp in Degree Celcius * 100 (uint16_t)
+5-7: Fan Max Temp in Degree Celcius * 100 (uint16_t)
+7-8: Fan Manual Override (bool)
+8-9: Fan Manual Speed (uint8_t)</t>
+  </si>
+  <si>
+    <t>Fan Settings</t>
+  </si>
+  <si>
+    <t>0-2: Update Interval Millis (uint16_t)
+2-4: Fan Off Temp in Degree Celcius * 100 (uint16_t)
+4-6: Fan Max Temp in Degree Celcius * 100 (uint16_t)
+6-7: Fan Manual Override (bool)
+7-8: Fan Manual Speed (uint8_t)</t>
+  </si>
+  <si>
+    <t>Motor-Fan Settings</t>
+  </si>
+  <si>
+    <t>RC Signals</t>
+  </si>
+  <si>
+    <t>RC Control Signals</t>
+  </si>
+  <si>
+    <t>0-2: Throttle Pulse Width in Microseconds
+2-4: Steering Pulse Width in Microseconds</t>
+  </si>
+  <si>
+    <t>RC-Receiver Input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,10 +204,10 @@
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -272,10 +275,6 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -284,14 +283,14 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1276349</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -351,13 +350,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -368,7 +367,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A348ECA3-17EA-4E04-8B77-A8BDE685592F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -418,81 +417,14 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{184C8A9B-2138-45F5-880D-0695FECD74F5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>28576</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -502,79 +434,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93B166A-BE8E-4ABA-B24C-6723F091E502}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>247649</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>1609724</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Check Box 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24002308-AC9D-47AE-8871-E468DDF37B69}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -628,10 +488,149 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F510DB-382D-42B4-8848-A6A4B301B15C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>247650</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>1609724</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>990600</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>542924</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -641,7 +640,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0506489-D8E3-447C-A899-AA86015C7AE4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -697,8 +696,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>247650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -708,7 +707,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3FE3FD4-63E9-4112-92A9-23D86D4BB8CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -759,90 +758,23 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>247649</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>409574</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2053"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{890BE3D8-1987-4287-BD5E-4E61DB6FE624}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1085850</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
+            <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2054"/>
+                  <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EA29E8B-3FB2-45BF-8F35-171BC80497E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32BBE23C-F394-4604-8B4D-4E30D44699A8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -890,28 +822,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D376CD15-575C-4A04-BFC7-316D307C4938}" name="Get" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{D4FD4796-7807-43B6-9C28-76F5D20D5DC2}" name="Write Argument1 (Index)" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A174D50D-1925-434C-A5D7-6B4AC9A58A0A}" name="Return (Bytes)" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4BD1E2F9-CE76-44BB-AA16-4AB7F8129EC2}" name="Return (Type)" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{823960EF-3E0B-40B7-921C-5C8CFC0B13A6}" name="Return (Description)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{65259A38-7403-4A76-A281-C4AE53A26E86}" name="Implemented" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D376CD15-575C-4A04-BFC7-316D307C4938}" name="Get" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{D4FD4796-7807-43B6-9C28-76F5D20D5DC2}" name="Write Argument1 (Index)" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{A174D50D-1925-434C-A5D7-6B4AC9A58A0A}" name="Return (Bytes)" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{4BD1E2F9-CE76-44BB-AA16-4AB7F8129EC2}" name="Return (Type)" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{823960EF-3E0B-40B7-921C-5C8CFC0B13A6}" name="Return (Description)" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{65259A38-7403-4A76-A281-C4AE53A26E86}" name="Implemented" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9EB8AAA-A541-4ECE-BFF1-8D9654029A1B}" name="Tabelle13" displayName="Tabelle13" ref="B3:G8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9EB8AAA-A541-4ECE-BFF1-8D9654029A1B}" name="Tabelle13" displayName="Tabelle13" ref="B3:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{979B0D7E-BC19-41CE-8B50-3452D4698604}" name="Set" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{6619177A-C347-431A-A484-FB8610E05981}" name="Write Argument2 (Bytes)" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{0E92F712-703E-46F5-8482-434A6F2C927F}" name="Write Argument2 (Type)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{ABC20142-4A43-4AF7-AA87-35F3900F9050}" name="Write Argument2 (Description)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4AC54CF2-3C35-48AB-8115-8972AF66ED03}" name="Implemented" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{979B0D7E-BC19-41CE-8B50-3452D4698604}" name="Set" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index)" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6619177A-C347-431A-A484-FB8610E05981}" name="Write Argument2 (Bytes)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{0E92F712-703E-46F5-8482-434A6F2C927F}" name="Write Argument2 (Type)" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{ABC20142-4A43-4AF7-AA87-35F3900F9050}" name="Write Argument2 (Description)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4AC54CF2-3C35-48AB-8115-8972AF66ED03}" name="Implemented" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1217,9 +1149,9 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B3:G8"/>
+  <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1229,7 +1161,7 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
@@ -1244,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1256,87 +1188,80 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1354,8 +1279,52 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>1276350</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId6" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
@@ -1370,63 +1339,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+            <control shapeId="1030" r:id="rId7" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId6" name="Check Box 3">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId7" name="Check Box 4">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1445,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DEAA1E-FBDA-4C3F-A80A-C706FE8B46C4}">
-  <dimension ref="B3:G8"/>
+  <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1382,7 @@
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="6" max="6" width="48.5703125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1466,24 +1391,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -1492,84 +1417,88 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
+    <row r="7" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1608,14 +1537,14 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>1609725</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>542925</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1636,8 +1565,8 @@
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>247650</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1646,42 +1575,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2053" r:id="rId6" name="Check Box 5">
+            <control shapeId="2055" r:id="rId6" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>247650</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>409575</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId7" name="Check Box 6">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>1085850</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1692,7 +1599,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished I2CManager commands started with StateManager
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Arduino\projects\AICar-RCController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281BB22F-1855-4DC2-8A92-26A27D415FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2425B8C4-2E1D-46ED-AFED-C7438688121E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
+    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C Get Commands" sheetId="1" r:id="rId1"/>
     <sheet name="I2C Set Commands" sheetId="2" r:id="rId2"/>
+    <sheet name="Status Led" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Get</t>
   </si>
@@ -97,14 +100,6 @@
   </si>
   <si>
     <t>Fan Info</t>
-  </si>
-  <si>
-    <t>0-1: Fan Speed (uint8_t)
-1-3: Update Interval Millis (uint16_t)
-3-5: Fan Off Temp in Degree Celcius * 100 (uint16_t)
-5-7: Fan Max Temp in Degree Celcius * 100 (uint16_t)
-7-8: Fan Manual Override (bool)
-8-9: Fan Manual Speed (uint8_t)</t>
   </si>
   <si>
     <t>Fan Settings</t>
@@ -132,15 +127,41 @@
   <si>
     <t>RC-Receiver Input</t>
   </si>
+  <si>
+    <t>Write Argument1 (Index - HIGHEST BIT SET)</t>
+  </si>
+  <si>
+    <t>0-1: Fan Speed (uint8_t)
+1-3: Update Interval Millis (uint16_t)
+3-5: Fan Off Temp in Degree Celcius * 100 (int16_t)
+5-7: Fan Max Temp in Degree Celcius * 100 (int16_t)
+7-8: Fan Manual Override (bool)
+8-9: Fan Manual Speed (uint8_t)</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +202,10 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -204,10 +228,10 @@
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -268,10 +292,6 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -290,7 +310,7 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1276349</xdr:rowOff>
+          <xdr:rowOff>1276350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -501,7 +521,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F510DB-382D-42B4-8848-A6A4B301B15C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -562,8 +582,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>1609725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -624,13 +644,13 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>1609724</xdr:rowOff>
+          <xdr:rowOff>1609725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>542924</xdr:rowOff>
+          <xdr:rowOff>542925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -689,82 +709,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>247650</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>1085850</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -774,7 +727,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32BBE23C-F394-4604-8B4D-4E30D44699A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -822,7 +775,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D376CD15-575C-4A04-BFC7-316D307C4938}" name="Get" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{D4FD4796-7807-43B6-9C28-76F5D20D5DC2}" name="Write Argument1 (Index)" dataDxfId="13"/>
@@ -839,13 +792,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9EB8AAA-A541-4ECE-BFF1-8D9654029A1B}" name="Tabelle13" displayName="Tabelle13" ref="B3:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{979B0D7E-BC19-41CE-8B50-3452D4698604}" name="Set" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index - HIGHEST BIT SET)" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{6619177A-C347-431A-A484-FB8610E05981}" name="Write Argument2 (Bytes)" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{0E92F712-703E-46F5-8482-434A6F2C927F}" name="Write Argument2 (Type)" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{ABC20142-4A43-4AF7-AA87-35F3900F9050}" name="Write Argument2 (Description)" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{4AC54CF2-3C35-48AB-8115-8972AF66ED03}" name="Implemented" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37ECAD0D-E8FA-4F5D-815A-DE15D8A1E4B6}" name="Tabelle3" displayName="Tabelle3" ref="B2:D8" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9151DA07-24AD-4DE1-909A-34A8DD2A01C4}" name="Color"/>
+    <tableColumn id="2" xr3:uid="{41143508-3CFA-433B-BC8A-9E1CA4EE079F}" name="Pulse"/>
+    <tableColumn id="3" xr3:uid="{4E0EE1F0-4EAC-48A5-8315-DC79A1183E9A}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1152,13 +1116,13 @@
   <dimension ref="B3:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
@@ -1211,7 +1175,7 @@
     </row>
     <row r="5" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -1220,10 +1184,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1241,7 +1205,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1264,6 +1228,7 @@
       <c r="G7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1372,14 +1337,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DEAA1E-FBDA-4C3F-A80A-C706FE8B46C4}">
   <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.5703125" customWidth="1"/>
@@ -1391,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -1426,7 +1391,7 @@
     </row>
     <row r="5" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1435,16 +1400,16 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -1453,10 +1418,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1553,42 +1518,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId5" name="Check Box 3">
+            <control shapeId="2055" r:id="rId5" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>247650</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2055" r:id="rId6" name="Check Box 7">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>5</xdr:row>
+                    <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>990600</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>1085850</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1599,7 +1542,41 @@
     </mc:Choice>
   </mc:AlternateContent>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A157500-C8DD-4DF8-AF44-709732728CB4}">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished StateManager finished ConfirmSwitchMode finished RCMode finished AIMode added python i2c-master api updated Datasheet
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Arduino\projects\AICar-RCController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2425B8C4-2E1D-46ED-AFED-C7438688121E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C91EDD-16B8-4E31-9359-DE14DC1EE21C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{22232B84-F53F-4A1B-8F12-B809FF9419EA}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C Get Commands" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Get</t>
   </si>
@@ -70,11 +70,6 @@
     <t>uint8</t>
   </si>
   <si>
-    <t>0 = Stand-by-Mode
-1 = RC-Mode (Passthrough)
-2 = AI-Mode (Only external control)</t>
-  </si>
-  <si>
     <t>Request Mode of Operation</t>
   </si>
   <si>
@@ -88,12 +83,6 @@
   </si>
   <si>
     <t>Implemented</t>
-  </si>
-  <si>
-    <t>0 = Stand-by-Mode
-1 = RC-Mode (Passthrough)
-2 = AI-Mode (Only external control)
-Timeout of 10 seconds to confirm the mode change via user input. (hold full brake and full left for at least 1 second and then relase to confirm)</t>
   </si>
   <si>
     <t>Motor Fan Info</t>
@@ -139,13 +128,67 @@
 8-9: Fan Manual Speed (uint8_t)</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Pulse</t>
-  </si>
-  <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>0 = Confirm-Switch-Mode
+1 = Stand-by-Mode
+2 = RC-Mode (Passthrough)
+3 = AI-Mode (Only external control)</t>
+  </si>
+  <si>
+    <t>Standby</t>
+  </si>
+  <si>
+    <t>RC-Mode</t>
+  </si>
+  <si>
+    <t>LED Color</t>
+  </si>
+  <si>
+    <t>LED Pulse</t>
+  </si>
+  <si>
+    <t>AI-Mode</t>
+  </si>
+  <si>
+    <t>Slow Flashing</t>
+  </si>
+  <si>
+    <t>RC-Mode Confirmation</t>
+  </si>
+  <si>
+    <t>AI-Mode Confirmation</t>
+  </si>
+  <si>
+    <t>Fast Flashing</t>
+  </si>
+  <si>
+    <t>AI-Mode Confirmation Complete, release controls to start</t>
+  </si>
+  <si>
+    <t>RC-Mode Confirmation Complete, release controls to start</t>
+  </si>
+  <si>
+    <t>Short Interval Flashing</t>
+  </si>
+  <si>
+    <t>Flashing</t>
+  </si>
+  <si>
+    <t>AI-Mode Cancelled by User Intervention</t>
+  </si>
+  <si>
+    <t>Mode Switch Confirmation Timeout</t>
+  </si>
+  <si>
+    <t>1 = Stand-by-Mode
+2 = RC-Mode (Passthrough)
+3 = AI-Mode (Only external control)
+Timeout of 10 seconds to confirm the mode change via user input. (hold full brake and full left for at least 1 second and then relase to confirm)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -167,12 +210,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -198,11 +271,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -256,6 +356,15 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,31 +377,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -309,8 +418,8 @@
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>1276350</xdr:rowOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -650,7 +759,7 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>542925</xdr:rowOff>
+          <xdr:rowOff>390525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -775,39 +884,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9E5DD71-BB2E-4EC7-BA06-EFB90C02DAE9}" name="Tabelle1" displayName="Tabelle1" ref="B3:G7" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D376CD15-575C-4A04-BFC7-316D307C4938}" name="Get" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D4FD4796-7807-43B6-9C28-76F5D20D5DC2}" name="Write Argument1 (Index)" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{A174D50D-1925-434C-A5D7-6B4AC9A58A0A}" name="Return (Bytes)" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{4BD1E2F9-CE76-44BB-AA16-4AB7F8129EC2}" name="Return (Type)" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{823960EF-3E0B-40B7-921C-5C8CFC0B13A6}" name="Return (Description)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{65259A38-7403-4A76-A281-C4AE53A26E86}" name="Implemented" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{D376CD15-575C-4A04-BFC7-316D307C4938}" name="Get" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{D4FD4796-7807-43B6-9C28-76F5D20D5DC2}" name="Write Argument1 (Index)" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{A174D50D-1925-434C-A5D7-6B4AC9A58A0A}" name="Return (Bytes)" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{4BD1E2F9-CE76-44BB-AA16-4AB7F8129EC2}" name="Return (Type)" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{823960EF-3E0B-40B7-921C-5C8CFC0B13A6}" name="Return (Description)" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{65259A38-7403-4A76-A281-C4AE53A26E86}" name="Implemented" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9EB8AAA-A541-4ECE-BFF1-8D9654029A1B}" name="Tabelle13" displayName="Tabelle13" ref="B3:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9EB8AAA-A541-4ECE-BFF1-8D9654029A1B}" name="Tabelle13" displayName="Tabelle13" ref="B3:G6" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{979B0D7E-BC19-41CE-8B50-3452D4698604}" name="Set" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index - HIGHEST BIT SET)" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6619177A-C347-431A-A484-FB8610E05981}" name="Write Argument2 (Bytes)" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0E92F712-703E-46F5-8482-434A6F2C927F}" name="Write Argument2 (Type)" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{ABC20142-4A43-4AF7-AA87-35F3900F9050}" name="Write Argument2 (Description)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4AC54CF2-3C35-48AB-8115-8972AF66ED03}" name="Implemented" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{979B0D7E-BC19-41CE-8B50-3452D4698604}" name="Set" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B7DC3677-DE9F-4BFD-A507-CC2EE05CACC7}" name="Write Argument1 (Index - HIGHEST BIT SET)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{6619177A-C347-431A-A484-FB8610E05981}" name="Write Argument2 (Bytes)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{0E92F712-703E-46F5-8482-434A6F2C927F}" name="Write Argument2 (Type)" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{ABC20142-4A43-4AF7-AA87-35F3900F9050}" name="Write Argument2 (Description)" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4AC54CF2-3C35-48AB-8115-8972AF66ED03}" name="Implemented" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37ECAD0D-E8FA-4F5D-815A-DE15D8A1E4B6}" name="Tabelle3" displayName="Tabelle3" ref="B2:D8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37ECAD0D-E8FA-4F5D-815A-DE15D8A1E4B6}" name="Tabelle3" displayName="Tabelle3" ref="B2:D11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9151DA07-24AD-4DE1-909A-34A8DD2A01C4}" name="Color"/>
-    <tableColumn id="2" xr3:uid="{41143508-3CFA-433B-BC8A-9E1CA4EE079F}" name="Pulse"/>
-    <tableColumn id="3" xr3:uid="{4E0EE1F0-4EAC-48A5-8315-DC79A1183E9A}" name="Description"/>
+    <tableColumn id="1" xr3:uid="{9151DA07-24AD-4DE1-909A-34A8DD2A01C4}" name="LED Color" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{41143508-3CFA-433B-BC8A-9E1CA4EE079F}" name="LED Pulse" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4E0EE1F0-4EAC-48A5-8315-DC79A1183E9A}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1115,8 +1224,8 @@
   </sheetPr>
   <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1152,15 +1261,15 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -1169,43 +1278,43 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1214,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -1250,8 +1359,8 @@
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>1276350</xdr:rowOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1338,7 +1447,7 @@
   <dimension ref="B3:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C32" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1356,24 +1465,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -1385,13 +1494,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1400,16 +1509,16 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -1418,10 +1527,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1509,7 +1618,7 @@
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>990600</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>542925</xdr:rowOff>
+                    <xdr:rowOff>390525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1549,28 +1658,119 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A157500-C8DD-4DF8-AF44-709732728CB4}">
-  <dimension ref="B2:D2"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>31</v>
-      </c>
+    </row>
+    <row r="5" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>